<commit_message>
Started adding passives for the new buiulding types.
</commit_message>
<xml_diff>
--- a/resources/data-imports/passive_skills.xlsx
+++ b/resources/data-imports/passive_skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>Leveling this skill will reduce the cost of units by 6% per level for a total of 30%. This reduces all resources, including gold and population.</t>
+  </si>
+  <si>
+    <t>Goblin Coin Bank</t>
+  </si>
+  <si>
+    <t>The goblins of Vax, an Island far off the south eastern cost of the Surface plane, have come to our lands to set up banks in your kingdoms. These banks can smelt your gold down to gold bars. Each kingdom you own that has this building may smelt up to 2 trillion (100 gold bars valued at 2 billion each) gold. Each bar adds 0.001 (or 0.1%) to your kingdoms defence for an additional 10% defence bonus.</t>
+  </si>
+  <si>
+    <t>Black Smiths Forge</t>
+  </si>
+  <si>
+    <t>As you level this skill you will unlock a new building, called Cannoneer Shop to create cannons for your kingdom that can also be deployed out to war. The higher this building level the less iron will be used through out the kingdom (up to 35%, 7% per level). This stacks with any cost reduction for the kingdom.</t>
+  </si>
+  <si>
+    <t>Cannoneer Shop</t>
+  </si>
+  <si>
+    <t>Create cannons for your army, these can be deployed like regular units and move much slower than Trebuchets. These can do devastating damage. When it comes to a kingdoms defence, they can only defend at 65% of their bonus defence against cannons and only 25% for walls against cannons.</t>
   </si>
 </sst>
 </file>
@@ -413,7 +431,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,7 +440,7 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="353" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="473" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="18" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="18" bestFit="true" customWidth="true" style="0"/>
@@ -510,9 +528,6 @@
       <c r="H3">
         <v>2</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
@@ -539,9 +554,6 @@
       <c r="H4">
         <v>4</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
@@ -568,9 +580,6 @@
       <c r="H5">
         <v>5</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
@@ -597,7 +606,91 @@
       <c r="H6">
         <v>5</v>
       </c>
-      <c r="I6">
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0.07</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New skill tree in place for passives
</commit_message>
<xml_diff>
--- a/resources/data-imports/passive_skills.xlsx
+++ b/resources/data-imports/passive_skills.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EB282A-7929-424B-8414-23EBD0C3AF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Passive Skills" sheetId="1" r:id="rId4"/>
+    <sheet name="Passive Skills" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -93,19 +109,26 @@
   </si>
   <si>
     <t>Create cannons for your army, these can be deployed like regular units and move much slower than Trebuchets. These can do devastating damage. When it comes to a kingdoms defence, they can only defend at 65% of their bonus defence against cannons and only 25% for walls against cannons.</t>
+  </si>
+  <si>
+    <t>Farmers Guild</t>
+  </si>
+  <si>
+    <t>At level 5, and not before, you will get, at hourly reset, 100% of your maximum population as you have learned how to use food efficiently to feed your population.</t>
+  </si>
+  <si>
+    <t>Calvary Training Grounds</t>
+  </si>
+  <si>
+    <t>This will unlock the Calvary Training Grounds Building, allowing you to recruit Mounted Knights and Mounted Archers.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -116,28 +139,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -427,31 +459,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="473" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="473" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -502,8 +529,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -528,8 +558,14 @@
       <c r="H3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -554,8 +590,14 @@
       <c r="H4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -580,8 +622,14 @@
       <c r="H5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -606,8 +654,14 @@
       <c r="H6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -635,8 +689,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -650,7 +707,7 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -664,8 +721,11 @@
       <c r="I8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -693,19 +753,77 @@
       <c r="I9">
         <v>1</v>
       </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on integrating passives with kingdoms.
- Fixing issues and implemtning the new buildings and assigning the
  buildings to players in a non destructive way as well as making sure
aspects of the passive skill system is working.
</commit_message>
<xml_diff>
--- a/resources/data-imports/passive_skills.xlsx
+++ b/resources/data-imports/passive_skills.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EB282A-7929-424B-8414-23EBD0C3AF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13791667-86EA-CA4F-8372-BAFF375E6D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -81,12 +81,6 @@
     <t>Leveling this skill will reduce the cost, be it gold or resources, needed to upgrade the building by 6% per level for a total of 30%. This skill will unlock Building Research</t>
   </si>
   <si>
-    <t>Building Research</t>
-  </si>
-  <si>
-    <t>This skill will allow you to create blue prints which are randomly rolled building details for new buildings that you can add to your kingdoms. You will also unlock the ability to create these blue prints as well as refine them. As you level this skill you get 5% towards refining for a total of 30%</t>
-  </si>
-  <si>
     <t>Unit Management</t>
   </si>
   <si>
@@ -114,7 +108,7 @@
     <t>Farmers Guild</t>
   </si>
   <si>
-    <t>At level 5, and not before, you will get, at hourly reset, 100% of your maximum population as you have learned how to use food efficiently to feed your population.</t>
+    <t>As you level this skill over time, you will reduce the population cost across the kingdom by 7% (Max: 35%). This only applies when you are using resources to acquire units and upgrade buildings. This will stack with other cost reduction passives.</t>
   </si>
   <si>
     <t>Calvary Training Grounds</t>
@@ -460,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -561,9 +555,6 @@
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -593,9 +584,6 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -608,25 +596,22 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>5</v>
       </c>
       <c r="I5">
         <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -637,28 +622,25 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="E6">
-        <v>0.06</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
       <c r="I6">
         <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -669,28 +651,25 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I7">
         <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -701,28 +680,25 @@
         <v>23</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I8">
         <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -733,28 +709,25 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I9">
         <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -765,10 +738,10 @@
         <v>27</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -777,48 +750,13 @@
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I10">
         <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>